<commit_message>
por hoje e so
</commit_message>
<xml_diff>
--- a/Comandos HTML-CSS-JS.xlsx
+++ b/Comandos HTML-CSS-JS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Desktop\Cursos\Curso-em-video-HTML-CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2B2B0F-2AA3-4BDC-90CD-BD42D3FA7CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB3D194-50E2-43EA-9373-88C742F37746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="165" windowWidth="9855" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HTML" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="592">
   <si>
     <t>Descrição</t>
   </si>
@@ -1843,6 +1843,69 @@
   </si>
   <si>
     <t>referrerpolicy="no-referrer" não ira caputar informação do iframe</t>
+  </si>
+  <si>
+    <t>            width: 0px;</t>
+  </si>
+  <si>
+    <t>            height: 0px;</t>
+  </si>
+  <si>
+    <t>para esconder a barra de rolagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">::-webkit-scrollbar{ </t>
+  </si>
+  <si>
+    <t>FORMULARIO</t>
+  </si>
+  <si>
+    <t>Botão de enviar</t>
+  </si>
+  <si>
+    <t>caixa de texto</t>
+  </si>
+  <si>
+    <t>&lt;input type="text" name="nome" id="nome"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input type="submit" value="Enviar"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form&gt; formulario entre na tag&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form autocomplete="off"&gt;</t>
+  </si>
+  <si>
+    <t>para não aparecer caixa de sugestão no input</t>
+  </si>
+  <si>
+    <t> &lt;form action="cadastro.php"&gt;</t>
+  </si>
+  <si>
+    <t>para fazer ligação com php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;label for="inome"&gt;Nome:&lt;/label&gt; </t>
+  </si>
+  <si>
+    <t>            &lt;input type="text" name="nome" id="inome" placeholder="Nome"&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>o FOR tem que ser o memo do ID</t>
+  </si>
+  <si>
+    <t>&lt;form method="get"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form method="post"&gt;</t>
+  </si>
+  <si>
+    <t>aparece os dados na url - só enviar a te 3 mil bytes maios ou mesmos 3000 mil letras (não pode usar em campo sensível senha/numero de cartao de credito/ envio de foto)</t>
+  </si>
+  <si>
+    <t>Não aparece os dados na url / pode ser usador mais de 3 mil bytes/ pode ser usado para senha/ cartao de credito/ e enviar arquivos, fotos.</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2366,7 +2429,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2568,8 +2630,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
@@ -2580,7 +2649,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3055,10 +3124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D260"/>
+  <dimension ref="A1:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,100 +3137,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3172,498 +3241,498 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="88" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="12"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="36" t="s">
         <v>512</v>
       </c>
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="90" t="s">
         <v>513</v>
       </c>
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="36" t="s">
         <v>514</v>
       </c>
-      <c r="B46" s="91"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-    </row>
-    <row r="47" spans="1:4" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="56" t="s">
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+    </row>
+    <row r="47" spans="1:4" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="55" t="s">
         <v>515</v>
       </c>
-      <c r="B47" s="91" t="s">
+      <c r="B47" s="90" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+    <row r="48" spans="1:4" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="55" t="s">
         <v>516</v>
       </c>
-      <c r="B48" s="91" t="s">
+      <c r="B48" s="90" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+    <row r="49" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="55" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+    <row r="50" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="55" t="s">
         <v>535</v>
       </c>
-      <c r="B50" s="91" t="s">
+      <c r="B50" s="90" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
+    <row r="51" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="55" t="s">
         <v>538</v>
       </c>
-      <c r="B51" s="91" t="s">
+      <c r="B51" s="90" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-    </row>
-    <row r="53" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
+    <row r="52" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="55"/>
+    </row>
+    <row r="53" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="55" t="s">
         <v>545</v>
       </c>
-      <c r="B53" s="91" t="s">
+      <c r="B53" s="90" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
+    <row r="54" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="55" t="s">
         <v>546</v>
       </c>
-      <c r="B54" s="91" t="s">
+      <c r="B54" s="90" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="56" t="s">
+    <row r="55" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="55" t="s">
         <v>549</v>
       </c>
-      <c r="B55" s="91" t="s">
+      <c r="B55" s="90" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
+    <row r="56" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="55" t="s">
         <v>551</v>
       </c>
-      <c r="B56" s="91" t="s">
+      <c r="B56" s="90" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-    </row>
-    <row r="58" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="56"/>
-    </row>
-    <row r="59" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-    </row>
-    <row r="60" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="84" t="s">
+    <row r="57" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+    </row>
+    <row r="58" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="55"/>
+    </row>
+    <row r="59" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="55"/>
+    </row>
+    <row r="60" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="83" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="86" t="s">
+    <row r="61" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="85" t="s">
         <v>541</v>
       </c>
-      <c r="B61" s="91" t="s">
+      <c r="B61" s="90" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
-    </row>
-    <row r="63" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="84" t="s">
+    <row r="62" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="55"/>
+    </row>
+    <row r="63" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="83" t="s">
         <v>542</v>
       </c>
-      <c r="B63" s="91" t="s">
+      <c r="B63" s="90" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="86" t="s">
+    <row r="64" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="85" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="56"/>
-    </row>
-    <row r="66" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56"/>
-    </row>
-    <row r="67" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="84" t="s">
+    <row r="65" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="55"/>
+    </row>
+    <row r="66" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="55"/>
+    </row>
+    <row r="67" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="83" t="s">
         <v>528</v>
       </c>
-      <c r="B67" s="91" t="s">
+      <c r="B67" s="90" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="85" t="s">
+    <row r="68" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="84" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="85" t="s">
+    <row r="69" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="84" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="86" t="s">
+    <row r="70" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="85" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="56"/>
-    </row>
-    <row r="72" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="84" t="s">
+    <row r="71" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="55"/>
+    </row>
+    <row r="72" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="83" t="s">
         <v>524</v>
       </c>
-      <c r="B72" s="91" t="s">
+      <c r="B72" s="90" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="86" t="s">
+    <row r="73" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="85" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="56"/>
-    </row>
-    <row r="75" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="84" t="s">
+    <row r="74" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="55"/>
+    </row>
+    <row r="75" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="83" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="91" t="s">
+      <c r="B75" s="90" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="86" t="s">
+    <row r="76" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="85" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="77" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="56"/>
-    </row>
-    <row r="78" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="56" t="s">
+    <row r="77" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="55"/>
+    </row>
+    <row r="78" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="55" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="56" t="s">
+    <row r="79" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="55" t="s">
         <v>555</v>
       </c>
-      <c r="B79" s="91" t="s">
+      <c r="B79" s="90" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="91" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="56" t="s">
+    <row r="80" spans="1:2" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="55" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="11" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A82" s="28" t="s">
+      <c r="A82" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="11" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B83" s="11" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B84" s="12"/>
+      <c r="B84" s="11"/>
     </row>
     <row r="85" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A85" s="28" t="s">
+      <c r="A85" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B86" s="12"/>
+      <c r="B86" s="11"/>
     </row>
     <row r="87" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B87" s="12"/>
+      <c r="B87" s="11"/>
     </row>
     <row r="88" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A88" s="28" t="s">
+      <c r="A88" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B88" s="12"/>
+      <c r="B88" s="11"/>
     </row>
     <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="28" t="s">
+      <c r="A89" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="56" t="s">
+      <c r="B89" s="55" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B90" s="12"/>
+      <c r="B90" s="11"/>
     </row>
     <row r="91" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A91" s="28" t="s">
+      <c r="A91" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B91" s="12"/>
+      <c r="B91" s="11"/>
     </row>
     <row r="92" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B92" s="12"/>
+      <c r="B92" s="11"/>
     </row>
     <row r="93" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A93" s="28" t="s">
+      <c r="A93" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="12"/>
+      <c r="B93" s="11"/>
     </row>
     <row r="94" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="12"/>
+      <c r="B94" s="11"/>
     </row>
     <row r="95" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B95" s="12"/>
+      <c r="B95" s="11"/>
     </row>
     <row r="96" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B96" s="12"/>
+      <c r="B96" s="11"/>
     </row>
     <row r="97" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B97" s="12"/>
+      <c r="B97" s="11"/>
     </row>
     <row r="98" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A98" s="28" t="s">
+      <c r="A98" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B98" s="12"/>
+      <c r="B98" s="11"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
+      <c r="A99" s="27" t="s">
         <v>123</v>
       </c>
       <c r="B99" t="s">
@@ -3671,742 +3740,840 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B100" s="12"/>
+      <c r="B100" s="11"/>
     </row>
     <row r="101" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B101" s="12"/>
+      <c r="B101" s="11"/>
     </row>
     <row r="102" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B102" s="12"/>
+      <c r="B102" s="11"/>
     </row>
     <row r="103" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A103" s="29" t="s">
+      <c r="A103" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="11" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A104" s="13"/>
-      <c r="B104" s="12"/>
+      <c r="A104" s="12"/>
+      <c r="B104" s="11"/>
     </row>
     <row r="105" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B105" s="33" t="s">
+      <c r="B105" s="32" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A106" s="31" t="s">
+      <c r="A106" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B106" s="12"/>
+      <c r="B106" s="11"/>
     </row>
     <row r="107" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A107" s="31" t="s">
+      <c r="A107" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B107" s="12"/>
+      <c r="B107" s="11"/>
     </row>
     <row r="108" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A108" s="31" t="s">
+      <c r="A108" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="B108" s="12"/>
+      <c r="B108" s="11"/>
     </row>
     <row r="109" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A109" s="31" t="s">
+      <c r="A109" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="B109" s="12"/>
+      <c r="B109" s="11"/>
     </row>
     <row r="110" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A110" s="31" t="s">
+      <c r="A110" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B110" s="12"/>
+      <c r="B110" s="11"/>
     </row>
     <row r="111" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A111" s="31" t="s">
+      <c r="A111" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B111" s="12"/>
+      <c r="B111" s="11"/>
     </row>
     <row r="112" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A112" s="31" t="s">
+      <c r="A112" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="B112" s="12"/>
+      <c r="B112" s="11"/>
     </row>
     <row r="113" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A113" s="31" t="s">
+      <c r="A113" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B113" s="12"/>
+      <c r="B113" s="11"/>
     </row>
     <row r="114" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A114" s="31" t="s">
+      <c r="A114" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="B114" s="12"/>
+      <c r="B114" s="11"/>
     </row>
     <row r="115" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A115" s="31" t="s">
+      <c r="A115" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B115" s="12"/>
+      <c r="B115" s="11"/>
     </row>
     <row r="116" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A116" s="32" t="s">
+      <c r="A116" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B116" s="12"/>
+      <c r="B116" s="11"/>
     </row>
     <row r="117" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="13"/>
-      <c r="B117" s="12"/>
+      <c r="A117" s="12"/>
+      <c r="B117" s="11"/>
     </row>
     <row r="118" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A118" s="13"/>
-      <c r="B118" s="12"/>
+      <c r="A118" s="12"/>
+      <c r="B118" s="11"/>
     </row>
     <row r="119" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
     </row>
     <row r="120" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B121" s="12" t="s">
+      <c r="B121" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A122" s="12" t="s">
+      <c r="A122" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B122" s="12" t="s">
+      <c r="B122" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A123" s="12" t="s">
+      <c r="A123" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B123" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B124" s="12" t="s">
+      <c r="B124" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="12" t="s">
+      <c r="A125" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B125" s="12" t="s">
+      <c r="B125" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A126" s="12" t="s">
+      <c r="A126" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B126" s="12" t="s">
+      <c r="B126" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A131" s="18" t="s">
+      <c r="A131" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B131" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A132" s="14" t="s">
+      <c r="A132" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B132" s="15">
+      <c r="B132" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A133" s="14" t="s">
+      <c r="A133" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B133" s="15">
+      <c r="B133" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A134" s="14" t="s">
+      <c r="A134" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B134" s="16">
+      <c r="B134" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A135" s="17" t="s">
+      <c r="A135" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B135" s="12"/>
+      <c r="B135" s="11"/>
     </row>
     <row r="136" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A136" s="12"/>
-      <c r="B136" s="12"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="11"/>
     </row>
     <row r="137" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
     </row>
     <row r="141" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B142" s="12" t="s">
+      <c r="B142" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A143" s="18" t="s">
+      <c r="A143" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B143" s="12"/>
+      <c r="B143" s="11"/>
     </row>
     <row r="144" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A144" s="14" t="s">
+      <c r="A144" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B144" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A145" s="14" t="s">
+      <c r="A145" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B145" s="12"/>
+      <c r="B145" s="11"/>
     </row>
     <row r="146" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A146" s="14" t="s">
+      <c r="A146" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B146" s="12"/>
+      <c r="B146" s="11"/>
     </row>
     <row r="147" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A147" s="14" t="s">
+      <c r="A147" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B147" s="12"/>
+      <c r="B147" s="11"/>
     </row>
     <row r="148" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A148" s="17" t="s">
+      <c r="A148" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B148" s="12"/>
+      <c r="B148" s="11"/>
     </row>
     <row r="153" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A153" s="7" t="s">
+      <c r="A153" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A154" s="12" t="s">
+      <c r="A154" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B154" s="12"/>
+      <c r="B154" s="11"/>
     </row>
     <row r="155" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A155" s="18" t="s">
+      <c r="A155" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B155" s="12"/>
+      <c r="B155" s="11"/>
     </row>
     <row r="156" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A156" s="14" t="s">
+      <c r="A156" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B156" s="12" t="s">
+      <c r="B156" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A157" s="14" t="s">
+      <c r="A157" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B157" s="12" t="s">
+      <c r="B157" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A158" s="14" t="s">
+      <c r="A158" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B158" s="12"/>
+      <c r="B158" s="11"/>
     </row>
     <row r="159" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A159" s="17" t="s">
+      <c r="A159" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B159" s="12"/>
+      <c r="B159" s="11"/>
     </row>
     <row r="160" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A160" s="12"/>
-      <c r="B160" s="12"/>
+      <c r="A160" s="11"/>
+      <c r="B160" s="11"/>
     </row>
     <row r="161" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A161" s="19" t="s">
+      <c r="A161" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B161" s="20"/>
+      <c r="B161" s="19"/>
     </row>
     <row r="162" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A162" s="21" t="s">
+      <c r="A162" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B162" s="22" t="s">
+      <c r="B162" s="21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A165" s="92" t="s">
+      <c r="A165" s="6" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A166" s="47" t="s">
+      <c r="A166" s="46" t="s">
         <v>557</v>
       </c>
-      <c r="B166" s="12" t="s">
+      <c r="B166" s="11" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A167" s="47"/>
-      <c r="B167" s="12"/>
+      <c r="A167" s="46"/>
+      <c r="B167" s="11"/>
     </row>
     <row r="168" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A168" s="56" t="s">
+      <c r="A168" s="55" t="s">
         <v>562</v>
       </c>
-      <c r="B168" s="12" t="s">
+      <c r="B168" s="11" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A169" s="47"/>
-      <c r="B169" s="12"/>
+      <c r="A169" s="46"/>
+      <c r="B169" s="11"/>
     </row>
     <row r="170" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A170" s="44" t="s">
+      <c r="A170" s="43" t="s">
         <v>559</v>
       </c>
-      <c r="B170" s="12" t="s">
+      <c r="B170" s="11" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A171" s="46" t="s">
+      <c r="A171" s="45" t="s">
         <v>560</v>
       </c>
-      <c r="B171" s="12"/>
+      <c r="B171" s="11"/>
     </row>
     <row r="172" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A172" s="47"/>
-      <c r="B172" s="12"/>
+      <c r="A172" s="46"/>
+      <c r="B172" s="11"/>
     </row>
     <row r="173" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A173" s="56" t="s">
+      <c r="A173" s="55" t="s">
         <v>567</v>
       </c>
-      <c r="B173" s="12" t="s">
+      <c r="B173" s="11" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A174" s="12"/>
-      <c r="B174" s="12"/>
+      <c r="A174" s="11"/>
+      <c r="B174" s="11"/>
     </row>
     <row r="175" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A175" s="56" t="s">
+      <c r="A175" s="55" t="s">
         <v>569</v>
       </c>
-      <c r="B175" s="12" t="s">
+      <c r="B175" s="11" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A176" s="12"/>
-      <c r="B176" s="12"/>
-    </row>
-    <row r="177" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A177" s="12"/>
-      <c r="B177" s="12"/>
-    </row>
-    <row r="178" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A178" s="12"/>
-      <c r="B178" s="12"/>
-    </row>
-    <row r="179" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A179" s="12"/>
-      <c r="B179" s="12"/>
-    </row>
-    <row r="180" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A180" s="12"/>
-      <c r="B180" s="12"/>
-    </row>
-    <row r="181" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A181" s="12"/>
-      <c r="B181" s="12"/>
-    </row>
-    <row r="182" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A182" s="93" t="s">
+      <c r="A176" s="11"/>
+      <c r="B176" s="11"/>
+    </row>
+    <row r="177" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A177" s="11"/>
+      <c r="B177" s="11"/>
+    </row>
+    <row r="178" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A178" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B178" s="98"/>
+    </row>
+    <row r="179" spans="1:2" s="90" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A179" s="36" t="s">
+        <v>580</v>
+      </c>
+      <c r="B179" s="89"/>
+    </row>
+    <row r="180" spans="1:2" s="90" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A180" s="36" t="s">
+        <v>581</v>
+      </c>
+      <c r="B180" s="89" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A181" s="36" t="s">
+        <v>579</v>
+      </c>
+      <c r="B181" s="11" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A182" s="36" t="s">
+        <v>578</v>
+      </c>
+      <c r="B182" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A183" s="36" t="s">
+        <v>583</v>
+      </c>
+      <c r="B183" s="11" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A184" s="11"/>
+      <c r="B184" s="11"/>
+    </row>
+    <row r="185" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A185" s="92" t="s">
+        <v>585</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A186" s="94" t="s">
+        <v>586</v>
+      </c>
+      <c r="B186" s="11"/>
+    </row>
+    <row r="187" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A187" s="11"/>
+      <c r="B187" s="11"/>
+    </row>
+    <row r="188" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A188" s="36" t="s">
+        <v>588</v>
+      </c>
+      <c r="B188" s="11" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A189" s="36" t="s">
+        <v>589</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A190" s="11"/>
+      <c r="B190" s="11"/>
+    </row>
+    <row r="191" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A191" s="11"/>
+      <c r="B191" s="11"/>
+    </row>
+    <row r="192" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A192" s="11"/>
+      <c r="B192" s="11"/>
+    </row>
+    <row r="193" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A193" s="11"/>
+      <c r="B193" s="11"/>
+    </row>
+    <row r="194" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A194" s="11"/>
+      <c r="B194" s="11"/>
+    </row>
+    <row r="195" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A195" s="11"/>
+      <c r="B195" s="11"/>
+    </row>
+    <row r="196" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A196" s="11"/>
+      <c r="B196" s="11"/>
+    </row>
+    <row r="197" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A197" s="11"/>
+      <c r="B197" s="11"/>
+    </row>
+    <row r="198" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A198" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B182" s="93"/>
-      <c r="C182" s="93"/>
-      <c r="D182" s="93"/>
-    </row>
-    <row r="183" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A183" s="12" t="s">
+      <c r="B198" s="95"/>
+      <c r="C198" s="95"/>
+      <c r="D198" s="95"/>
+    </row>
+    <row r="199" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A199" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B183" s="12" t="s">
+      <c r="B199" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A184" s="12" t="s">
+    <row r="200" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A200" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B184" s="12" t="s">
+      <c r="B200" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A185" s="12" t="s">
+    <row r="201" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A201" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B185" s="12" t="s">
+      <c r="B201" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A186" s="12" t="s">
+    <row r="202" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A202" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B186" s="12" t="s">
+      <c r="B202" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A187" s="12" t="s">
+    <row r="203" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A203" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B187" s="12" t="s">
+      <c r="B203" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B188" s="12" t="s">
+    <row r="204" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B204" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="3" t="s">
+    <row r="209" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A209" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B193" s="1"/>
-    </row>
-    <row r="194" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A194" s="12" t="s">
+      <c r="B209" s="1"/>
+    </row>
+    <row r="210" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A210" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B194" s="12" t="s">
+      <c r="B210" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A195" s="12" t="s">
+    <row r="211" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A211" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B195" s="12" t="s">
+      <c r="B211" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A196" s="12" t="s">
+    <row r="212" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A212" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B196" s="12" t="s">
+      <c r="B212" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A199" s="5" t="s">
+    <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A215" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B199" s="24"/>
-    </row>
-    <row r="200" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A200" s="4" t="s">
+      <c r="B215" s="23"/>
+    </row>
+    <row r="216" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A216" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B216" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A206" s="8" t="s">
+    <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A222" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B206" s="9"/>
-    </row>
-    <row r="207" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A207" s="12" t="s">
+      <c r="B222" s="8"/>
+    </row>
+    <row r="223" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A223" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A208" s="12" t="s">
+    <row r="224" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A224" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A209" s="12" t="s">
+    <row r="225" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A225" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A210" s="12" t="s">
+    <row r="226" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A226" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A211" s="12" t="s">
+    <row r="227" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A227" s="11" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A212" s="12" t="s">
+    <row r="228" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A228" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="96" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="91" t="s">
         <v>564</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B229" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="96" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="91" t="s">
         <v>565</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B230" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A215" s="12"/>
-    </row>
-    <row r="216" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A216" s="12"/>
-    </row>
-    <row r="217" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A217" s="12"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="39" t="s">
+    <row r="231" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A231" s="11"/>
+    </row>
+    <row r="232" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A232" s="11"/>
+    </row>
+    <row r="233" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A233" s="11"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="38" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="40" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="39" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="41" t="s">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="40" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="41" t="s">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="40" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="41"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="41" t="s">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="40"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="40" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="41" t="s">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="40" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="41" t="s">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="40" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="42" t="s">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="41" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="41" t="s">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="40" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="41" t="s">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="40" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="41" t="s">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="40" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="41" t="s">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="40" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="43" t="s">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="42" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="37"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="37"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="37"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="37"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="37"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="37"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="37"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="37"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="37"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="37"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="37"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="37"/>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="37" t="s">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="36"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="36"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="36"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="36"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="36"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="36"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="36"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="36"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="36"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="36"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="36"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="36"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="36" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="37"/>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="37"/>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="37"/>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="37"/>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="37"/>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="37"/>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="37"/>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="37"/>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="38"/>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="38"/>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="37"/>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="37" t="s">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="36"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="36"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="36"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="36"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="36"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="36"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="36"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="36"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="37"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="37"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="36"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="36" t="s">
         <v>237</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A182:D182"/>
+    <mergeCell ref="A198:D198"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4415,10 +4582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF404A17-505C-47C1-BA5C-9EC05B6288D3}">
-  <dimension ref="A2:E143"/>
+  <dimension ref="A2:E146"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4428,610 +4595,610 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="12"/>
+      <c r="B35" s="11"/>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="12"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="12"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
     <row r="43" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="12"/>
+      <c r="B43" s="11"/>
     </row>
     <row r="44" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B47" s="12"/>
+      <c r="B47" s="11"/>
     </row>
     <row r="48" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="94" t="s">
+      <c r="A50" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="B50" s="94"/>
+      <c r="B50" s="96"/>
     </row>
     <row r="51" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="95" t="s">
+      <c r="A51" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="95"/>
+      <c r="B51" s="97"/>
     </row>
     <row r="52" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B53" s="12"/>
+      <c r="B53" s="11"/>
     </row>
     <row r="54" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="B58" s="12"/>
+      <c r="B58" s="11"/>
     </row>
     <row r="59" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="B59" s="12"/>
+      <c r="B59" s="11"/>
     </row>
     <row r="60" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A60" s="47"/>
-      <c r="B60" s="12"/>
-    </row>
-    <row r="61" spans="1:2" s="53" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A61" s="54" t="s">
+      <c r="A60" s="46"/>
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="1:2" s="52" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A61" s="53" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="44" t="s">
+      <c r="A62" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="11" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="45" t="s">
+      <c r="A64" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="B64" s="12"/>
+      <c r="B64" s="11"/>
     </row>
     <row r="65" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="45" t="s">
+      <c r="A65" s="44" t="s">
         <v>261</v>
       </c>
-      <c r="B65" s="12"/>
+      <c r="B65" s="11"/>
     </row>
     <row r="66" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A66" s="45" t="s">
+      <c r="A66" s="44" t="s">
         <v>262</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="11" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A67" s="45" t="s">
+      <c r="A67" s="44" t="s">
         <v>263</v>
       </c>
-      <c r="B67" s="12"/>
+      <c r="B67" s="11"/>
     </row>
     <row r="68" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="B68" s="12"/>
+      <c r="B68" s="11"/>
     </row>
     <row r="69" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A69" s="48"/>
-      <c r="B69" s="12"/>
+      <c r="A69" s="47"/>
+      <c r="B69" s="11"/>
     </row>
     <row r="70" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A70" s="47" t="s">
+      <c r="A70" s="46" t="s">
         <v>276</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="11" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A71" s="47" t="s">
+      <c r="A71" s="46" t="s">
         <v>277</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="11" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A72" s="47"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="46"/>
+      <c r="B72" s="11"/>
     </row>
     <row r="73" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A73" s="44" t="s">
+      <c r="A73" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="11" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A74" s="45" t="s">
+      <c r="A74" s="44" t="s">
         <v>272</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="11" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="B75" s="12"/>
+      <c r="B75" s="11"/>
     </row>
     <row r="76" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="46" t="s">
+      <c r="A76" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B76" s="12"/>
+      <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A77" s="50"/>
-      <c r="B77" s="12"/>
+      <c r="A77" s="49"/>
+      <c r="B77" s="11"/>
     </row>
     <row r="78" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A78" s="50" t="s">
+      <c r="A78" s="49" t="s">
         <v>293</v>
       </c>
-      <c r="B78" s="12"/>
+      <c r="B78" s="11"/>
     </row>
     <row r="80" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
+      <c r="A80" s="48" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A81" s="12" t="s">
+      <c r="A81" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="11" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="11" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B83" s="11" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B84" s="12"/>
+      <c r="B84" s="11"/>
     </row>
     <row r="85" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A87" s="12" t="s">
+      <c r="A87" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" s="11" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="11" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="11" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="B90" s="12" t="s">
+      <c r="B90" s="11" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A91" s="12" t="s">
+      <c r="A91" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="B91" s="12" t="s">
+      <c r="B91" s="11" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A92" s="56" t="s">
+      <c r="A92" s="55" t="s">
         <v>505</v>
       </c>
-      <c r="B92" s="12"/>
+      <c r="B92" s="11"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="56" t="s">
+      <c r="A93" s="55" t="s">
         <v>506</v>
       </c>
       <c r="B93" t="s">
@@ -5039,268 +5206,291 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A99" s="53" t="s">
+      <c r="A99" s="52" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B100" s="11" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="11" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
     </row>
     <row r="103" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B103" s="12"/>
+      <c r="B103" s="11"/>
     </row>
     <row r="104" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="B104" s="12" t="s">
+      <c r="B104" s="11" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A105" s="12" t="s">
+      <c r="A105" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="B105" s="12" t="s">
+      <c r="B105" s="11" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A106" s="12" t="s">
+      <c r="A106" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="B106" s="12" t="s">
+      <c r="B106" s="11" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="B107" s="51" t="s">
+      <c r="B107" s="50" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A108" s="12" t="s">
+      <c r="A108" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="11" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A109" s="12" t="s">
+      <c r="A109" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="B109" s="12" t="s">
+      <c r="B109" s="11" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="B110" s="12" t="s">
+      <c r="B110" s="11" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A113" s="53" t="s">
+      <c r="A113" s="52" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A114" s="12" t="s">
+      <c r="A114" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B114" s="11" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A115" s="12" t="s">
+      <c r="A115" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="B115" s="12" t="s">
+      <c r="B115" s="11" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A116" s="12" t="s">
+      <c r="A116" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="11" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B117" s="11" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A118" s="12" t="s">
+      <c r="A118" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="B118" s="11" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="B119" s="12" t="s">
+      <c r="B119" s="11" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A120" s="12" t="s">
+      <c r="A120" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="11" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A124" s="87" t="s">
+    <row r="121" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+    </row>
+    <row r="122" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A122" s="92" t="s">
+        <v>574</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A123" s="93" t="s">
+        <v>571</v>
+      </c>
+      <c r="B123" s="11"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="94" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A127" s="86" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="13" t="s">
+    <row r="128" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A128" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="B125" s="12"/>
-    </row>
-    <row r="126" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A126" s="13" t="s">
+      <c r="B128" s="11"/>
+    </row>
+    <row r="129" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A129" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="B126" s="12" t="s">
+      <c r="B129" s="11" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A127" s="13" t="s">
+    <row r="130" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A130" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="B127" s="12" t="s">
+      <c r="B130" s="11" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A128" s="13" t="s">
+    <row r="131" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A131" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="B131" s="11" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A129" s="56" t="s">
+    <row r="132" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A132" s="55" t="s">
         <v>502</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B132" s="11" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A130" s="13" t="s">
+    <row r="133" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A133" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B133" s="11" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A131" s="56" t="s">
+    <row r="134" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A134" s="55" t="s">
         <v>496</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B134" s="11" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A132" s="56" t="s">
+    <row r="135" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A135" s="55" t="s">
         <v>498</v>
       </c>
-      <c r="B132" s="12" t="s">
+      <c r="B135" s="11" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A133" s="56" t="s">
+    <row r="136" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A136" s="55" t="s">
         <v>502</v>
       </c>
-      <c r="B133" s="12" t="s">
+      <c r="B136" s="11" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A134" s="56" t="s">
+    <row r="137" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A137" s="55" t="s">
         <v>509</v>
       </c>
-      <c r="B134" s="12" t="s">
+      <c r="B137" s="11" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A135" s="90"/>
-      <c r="B135" s="12"/>
-    </row>
-    <row r="136" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A136" s="12"/>
-      <c r="B136" s="12"/>
-    </row>
-    <row r="137" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
-    </row>
     <row r="138" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
+      <c r="A138" s="89"/>
+      <c r="B138" s="11"/>
     </row>
     <row r="139" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
     </row>
     <row r="140" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
     </row>
     <row r="141" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
+      <c r="A141" s="11"/>
+      <c r="B141" s="11"/>
     </row>
     <row r="142" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
     </row>
     <row r="143" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A143" s="12"/>
-      <c r="B143" s="12"/>
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
+    </row>
+    <row r="144" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A144" s="11"/>
+      <c r="B144" s="11"/>
+    </row>
+    <row r="145" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A145" s="11"/>
+      <c r="B145" s="11"/>
+    </row>
+    <row r="146" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A146" s="11"/>
+      <c r="B146" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5327,7 +5517,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>500</v>
       </c>
       <c r="B4" t="s">
@@ -5368,12 +5558,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5427,7 +5617,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="54" t="s">
         <v>341</v>
       </c>
       <c r="B5" t="s">
@@ -5443,325 +5633,325 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="51" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="55" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="61" t="s">
         <v>359</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="59" t="s">
         <v>362</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="62" t="s">
         <v>364</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="64" t="s">
         <v>366</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="11"/>
     </row>
     <row r="23" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="59" t="s">
         <v>372</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="62" t="s">
         <v>364</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="63" t="s">
         <v>373</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="62" t="s">
         <v>375</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="62" t="s">
         <v>376</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="11"/>
     </row>
     <row r="32" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="63" t="s">
         <v>377</v>
       </c>
-      <c r="B32" s="12"/>
+      <c r="B32" s="11"/>
     </row>
     <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="36" t="s">
         <v>430</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="59" t="s">
         <v>432</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="63" t="s">
         <v>433</v>
       </c>
-      <c r="B40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="59" t="s">
         <v>432</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="64" t="s">
+      <c r="A43" s="63" t="s">
         <v>435</v>
       </c>
-      <c r="B43" s="12"/>
+      <c r="B43" s="11"/>
     </row>
     <row r="44" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="57"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="60" t="s">
+      <c r="A45" s="59" t="s">
         <v>436</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="B46" s="12"/>
+      <c r="B46" s="11"/>
     </row>
     <row r="47" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="11"/>
     </row>
     <row r="48" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="36" t="s">
         <v>439</v>
       </c>
-      <c r="B48" s="12"/>
+      <c r="B48" s="11"/>
     </row>
     <row r="49" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="76" t="s">
+      <c r="A49" s="75" t="s">
         <v>440</v>
       </c>
-      <c r="B49" s="12"/>
+      <c r="B49" s="11"/>
     </row>
     <row r="50" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A50" s="37"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="11"/>
     </row>
     <row r="51" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A51" s="78" t="s">
+      <c r="A51" s="77" t="s">
         <v>441</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A52" s="79" t="s">
+      <c r="A52" s="78" t="s">
         <v>442</v>
       </c>
-      <c r="B52" s="12"/>
+      <c r="B52" s="11"/>
     </row>
     <row r="53" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A53" s="80" t="s">
+      <c r="A53" s="79" t="s">
         <v>443</v>
       </c>
-      <c r="B53" s="12"/>
+      <c r="B53" s="11"/>
     </row>
     <row r="54" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A54" s="37"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="11"/>
     </row>
     <row r="55" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="78" t="s">
+      <c r="A55" s="77" t="s">
         <v>445</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A56" s="80" t="s">
+      <c r="A56" s="79" t="s">
         <v>446</v>
       </c>
-      <c r="B56" s="12"/>
+      <c r="B56" s="11"/>
     </row>
     <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="80" t="s">
         <v>447</v>
       </c>
       <c r="B58" t="s">
@@ -5769,15 +5959,15 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="82" t="s">
+      <c r="A59" s="81" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
+      <c r="A60" s="11"/>
     </row>
     <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="80" t="s">
         <v>452</v>
       </c>
       <c r="B61" t="s">
@@ -5785,31 +5975,31 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="82" t="s">
+      <c r="A62" s="81" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
+      <c r="A63" s="11"/>
       <c r="B63" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="81" t="s">
+      <c r="A64" s="80" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="82" t="s">
+      <c r="A65" s="81" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
+      <c r="A66" s="11"/>
     </row>
     <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="81" t="s">
+      <c r="A67" s="80" t="s">
         <v>457</v>
       </c>
       <c r="B67" t="s">
@@ -5817,67 +6007,67 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="83" t="s">
+      <c r="A68" s="82" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="82" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="83" t="s">
+      <c r="A70" s="82" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="83" t="s">
+      <c r="A71" s="82" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="83" t="s">
+      <c r="A72" s="82" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="83" t="s">
+      <c r="A73" s="82" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="83" t="s">
+      <c r="A74" s="82" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="83" t="s">
+      <c r="A75" s="82" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="83" t="s">
+      <c r="A76" s="82" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="83" t="s">
+      <c r="A77" s="82" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="82" t="s">
+      <c r="A78" s="81" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="56" t="s">
+      <c r="A79" s="55" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="84" t="s">
+      <c r="A80" s="83" t="s">
         <v>478</v>
       </c>
       <c r="B80" t="s">
@@ -5885,46 +6075,46 @@
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="85" t="s">
+      <c r="A81" s="84" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="85" t="s">
+      <c r="A82" s="84" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="85" t="s">
+      <c r="A83" s="84" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="85" t="s">
+      <c r="A84" s="84" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="86" t="s">
+      <c r="A85" s="85" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A134" s="57" t="s">
+      <c r="A134" s="56" t="s">
         <v>346</v>
       </c>
-      <c r="B134" s="12"/>
+      <c r="B134" s="11"/>
     </row>
     <row r="135" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A135" s="12" t="s">
+      <c r="A135" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="B135" s="12" t="s">
+      <c r="B135" s="11" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A136" s="12" t="s">
+      <c r="A136" s="11" t="s">
         <v>349</v>
       </c>
       <c r="B136" t="s">
@@ -5932,484 +6122,484 @@
       </c>
     </row>
     <row r="137" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A137" s="12" t="s">
+      <c r="A137" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="B137" s="12" t="s">
+      <c r="B137" s="11" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A138" s="12" t="s">
+      <c r="A138" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="B138" s="12" t="s">
+      <c r="B138" s="11" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A139" s="12" t="s">
+      <c r="A139" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B139" s="11" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
     </row>
     <row r="141" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
+      <c r="A141" s="11"/>
+      <c r="B141" s="11"/>
     </row>
     <row r="142" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A142" s="66" t="s">
+      <c r="A142" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="B142" s="67"/>
+      <c r="B142" s="66"/>
     </row>
     <row r="143" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A143" s="68" t="s">
+      <c r="A143" s="67" t="s">
         <v>367</v>
       </c>
-      <c r="B143" s="69" t="s">
+      <c r="B143" s="68" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="70" t="s">
+      <c r="A144" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="B144" s="71" t="s">
+      <c r="B144" s="70" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A145" s="73"/>
-      <c r="B145" s="73"/>
+      <c r="A145" s="72"/>
+      <c r="B145" s="72"/>
     </row>
     <row r="146" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A146" s="74" t="s">
+      <c r="A146" s="73" t="s">
         <v>384</v>
       </c>
-      <c r="B146" s="12"/>
+      <c r="B146" s="11"/>
     </row>
     <row r="147" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A147" s="12" t="s">
+      <c r="A147" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="B147" s="12" t="s">
+      <c r="B147" s="11" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A148" s="12" t="s">
+      <c r="A148" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="B148" s="12" t="s">
+      <c r="B148" s="11" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A149" s="12" t="s">
+      <c r="A149" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="B149" s="72" t="s">
+      <c r="B149" s="71" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A150" s="72"/>
-      <c r="B150" s="12"/>
+      <c r="A150" s="71"/>
+      <c r="B150" s="11"/>
     </row>
     <row r="151" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A151" s="12"/>
-      <c r="B151" s="12"/>
+      <c r="A151" s="11"/>
+      <c r="B151" s="11"/>
     </row>
     <row r="152" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A152" s="12"/>
-      <c r="B152" s="12"/>
+      <c r="A152" s="11"/>
+      <c r="B152" s="11"/>
     </row>
     <row r="153" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A153" s="12"/>
-      <c r="B153" s="12"/>
+      <c r="A153" s="11"/>
+      <c r="B153" s="11"/>
     </row>
     <row r="154" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A154" s="12"/>
-      <c r="B154" s="12"/>
+      <c r="A154" s="11"/>
+      <c r="B154" s="11"/>
     </row>
     <row r="155" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A155" s="12"/>
-      <c r="B155" s="12"/>
+      <c r="A155" s="11"/>
+      <c r="B155" s="11"/>
     </row>
     <row r="156" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A156" s="12"/>
-      <c r="B156" s="12"/>
+      <c r="A156" s="11"/>
+      <c r="B156" s="11"/>
     </row>
     <row r="157" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A157" s="12"/>
-      <c r="B157" s="12"/>
+      <c r="A157" s="11"/>
+      <c r="B157" s="11"/>
     </row>
     <row r="158" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A158" s="12"/>
-      <c r="B158" s="12"/>
+      <c r="A158" s="11"/>
+      <c r="B158" s="11"/>
     </row>
     <row r="159" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A159" s="12"/>
-      <c r="B159" s="12"/>
+      <c r="A159" s="11"/>
+      <c r="B159" s="11"/>
     </row>
     <row r="160" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A160" s="12"/>
-      <c r="B160" s="12"/>
+      <c r="A160" s="11"/>
+      <c r="B160" s="11"/>
     </row>
     <row r="161" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A161" s="12"/>
-      <c r="B161" s="12"/>
+      <c r="A161" s="11"/>
+      <c r="B161" s="11"/>
     </row>
     <row r="162" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A162" s="12"/>
-      <c r="B162" s="12"/>
+      <c r="A162" s="11"/>
+      <c r="B162" s="11"/>
     </row>
     <row r="163" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A163" s="12"/>
-      <c r="B163" s="12"/>
+      <c r="A163" s="11"/>
+      <c r="B163" s="11"/>
     </row>
     <row r="164" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A164" s="12"/>
-      <c r="B164" s="12"/>
+      <c r="A164" s="11"/>
+      <c r="B164" s="11"/>
     </row>
     <row r="165" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A165" s="12"/>
-      <c r="B165" s="12"/>
+      <c r="A165" s="11"/>
+      <c r="B165" s="11"/>
     </row>
     <row r="166" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A166" s="12"/>
-      <c r="B166" s="12"/>
+      <c r="A166" s="11"/>
+      <c r="B166" s="11"/>
     </row>
     <row r="167" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A167" s="12" t="s">
+      <c r="A167" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="B167" s="12"/>
+      <c r="B167" s="11"/>
     </row>
     <row r="168" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A168" s="12"/>
-      <c r="B168" s="12"/>
+      <c r="A168" s="11"/>
+      <c r="B168" s="11"/>
     </row>
     <row r="169" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A169" s="12"/>
-      <c r="B169" s="12"/>
+      <c r="A169" s="11"/>
+      <c r="B169" s="11"/>
     </row>
     <row r="170" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A170" s="75" t="s">
+      <c r="A170" s="74" t="s">
         <v>409</v>
       </c>
-      <c r="B170" s="12"/>
+      <c r="B170" s="11"/>
     </row>
     <row r="171" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A171" s="12" t="s">
+      <c r="A171" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="B171" s="12" t="s">
+      <c r="B171" s="11" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A172" s="12" t="s">
+      <c r="A172" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="11" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A173" s="12" t="s">
+      <c r="A173" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="B173" s="12" t="s">
+      <c r="B173" s="11" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A174" s="12" t="s">
+      <c r="A174" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="B174" s="12" t="s">
+      <c r="B174" s="11" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A175" s="12" t="s">
+      <c r="A175" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="B175" s="12"/>
+      <c r="B175" s="11"/>
     </row>
     <row r="176" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A176" s="12" t="s">
+      <c r="A176" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="B176" s="12" t="s">
+      <c r="B176" s="11" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A177" s="75" t="s">
+      <c r="A177" s="74" t="s">
         <v>387</v>
       </c>
-      <c r="B177" s="12"/>
+      <c r="B177" s="11"/>
     </row>
     <row r="178" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A178" s="12" t="s">
+      <c r="A178" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="B178" s="12" t="s">
+      <c r="B178" s="11" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A179" s="12" t="s">
+      <c r="A179" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="B179" s="12" t="s">
+      <c r="B179" s="11" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A180" s="12" t="s">
+      <c r="A180" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="11" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A181" s="12" t="s">
+      <c r="A181" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="B181" s="12" t="s">
+      <c r="B181" s="11" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A182" s="72" t="s">
+      <c r="A182" s="71" t="s">
         <v>392</v>
       </c>
-      <c r="B182" s="12" t="s">
+      <c r="B182" s="11" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A183" s="12" t="s">
+      <c r="A183" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="B183" s="12" t="s">
+      <c r="B183" s="11" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A184" s="12"/>
-      <c r="B184" s="12"/>
+      <c r="A184" s="11"/>
+      <c r="B184" s="11"/>
     </row>
     <row r="185" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A185" s="75" t="s">
+      <c r="A185" s="74" t="s">
         <v>400</v>
       </c>
-      <c r="B185" s="12"/>
+      <c r="B185" s="11"/>
     </row>
     <row r="186" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A186" s="12" t="s">
+      <c r="A186" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="B186" s="12" t="s">
+      <c r="B186" s="11" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A187" s="12" t="s">
+      <c r="A187" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="B187" s="12" t="s">
+      <c r="B187" s="11" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A188" s="12" t="s">
+      <c r="A188" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="B188" s="12" t="s">
+      <c r="B188" s="11" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A189" s="12"/>
-      <c r="B189" s="12"/>
+      <c r="A189" s="11"/>
+      <c r="B189" s="11"/>
     </row>
     <row r="190" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A190" s="12" t="s">
+      <c r="A190" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="B190" s="12"/>
+      <c r="B190" s="11"/>
     </row>
     <row r="191" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A191" s="12" t="s">
+      <c r="A191" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="B191" s="12"/>
+      <c r="B191" s="11"/>
     </row>
     <row r="192" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A192" s="12" t="s">
+      <c r="A192" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="B192" s="12"/>
+      <c r="B192" s="11"/>
     </row>
     <row r="193" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A193" s="12"/>
-      <c r="B193" s="12"/>
+      <c r="A193" s="11"/>
+      <c r="B193" s="11"/>
     </row>
     <row r="194" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A194" s="12"/>
-      <c r="B194" s="12"/>
+      <c r="A194" s="11"/>
+      <c r="B194" s="11"/>
     </row>
     <row r="195" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A195" s="12"/>
-      <c r="B195" s="12"/>
+      <c r="A195" s="11"/>
+      <c r="B195" s="11"/>
     </row>
     <row r="196" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A196" s="12"/>
-      <c r="B196" s="12"/>
+      <c r="A196" s="11"/>
+      <c r="B196" s="11"/>
     </row>
     <row r="197" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A197" s="12"/>
-      <c r="B197" s="12"/>
+      <c r="A197" s="11"/>
+      <c r="B197" s="11"/>
     </row>
     <row r="198" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A198" s="12"/>
-      <c r="B198" s="12"/>
+      <c r="A198" s="11"/>
+      <c r="B198" s="11"/>
     </row>
     <row r="199" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A199" s="12"/>
-      <c r="B199" s="12"/>
+      <c r="A199" s="11"/>
+      <c r="B199" s="11"/>
     </row>
     <row r="200" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A200" s="12"/>
-      <c r="B200" s="12"/>
+      <c r="A200" s="11"/>
+      <c r="B200" s="11"/>
     </row>
     <row r="201" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A201" s="12"/>
-      <c r="B201" s="12"/>
+      <c r="A201" s="11"/>
+      <c r="B201" s="11"/>
     </row>
     <row r="202" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A202" s="12"/>
-      <c r="B202" s="12"/>
+      <c r="A202" s="11"/>
+      <c r="B202" s="11"/>
     </row>
     <row r="203" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A203" s="12"/>
-      <c r="B203" s="12"/>
+      <c r="A203" s="11"/>
+      <c r="B203" s="11"/>
     </row>
     <row r="204" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A204" s="12"/>
-      <c r="B204" s="12"/>
+      <c r="A204" s="11"/>
+      <c r="B204" s="11"/>
     </row>
     <row r="205" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A205" s="12"/>
-      <c r="B205" s="12"/>
+      <c r="A205" s="11"/>
+      <c r="B205" s="11"/>
     </row>
     <row r="206" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A206" s="12"/>
-      <c r="B206" s="12"/>
+      <c r="A206" s="11"/>
+      <c r="B206" s="11"/>
     </row>
     <row r="207" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A207" s="12"/>
-      <c r="B207" s="12"/>
+      <c r="A207" s="11"/>
+      <c r="B207" s="11"/>
     </row>
     <row r="208" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A208" s="12"/>
-      <c r="B208" s="12"/>
+      <c r="A208" s="11"/>
+      <c r="B208" s="11"/>
     </row>
     <row r="209" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A209" s="12"/>
-      <c r="B209" s="12"/>
+      <c r="A209" s="11"/>
+      <c r="B209" s="11"/>
     </row>
     <row r="210" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A210" s="12"/>
-      <c r="B210" s="12"/>
+      <c r="A210" s="11"/>
+      <c r="B210" s="11"/>
     </row>
     <row r="211" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A211" s="12"/>
-      <c r="B211" s="12"/>
+      <c r="A211" s="11"/>
+      <c r="B211" s="11"/>
     </row>
     <row r="212" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A212" s="12"/>
-      <c r="B212" s="12"/>
+      <c r="A212" s="11"/>
+      <c r="B212" s="11"/>
     </row>
     <row r="213" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A213" s="12"/>
-      <c r="B213" s="12"/>
+      <c r="A213" s="11"/>
+      <c r="B213" s="11"/>
     </row>
     <row r="214" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A214" s="12"/>
-      <c r="B214" s="12"/>
+      <c r="A214" s="11"/>
+      <c r="B214" s="11"/>
     </row>
     <row r="215" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A215" s="12"/>
-      <c r="B215" s="12"/>
+      <c r="A215" s="11"/>
+      <c r="B215" s="11"/>
     </row>
     <row r="216" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A216" s="12"/>
-      <c r="B216" s="12"/>
+      <c r="A216" s="11"/>
+      <c r="B216" s="11"/>
     </row>
     <row r="217" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A217" s="12"/>
-      <c r="B217" s="12"/>
+      <c r="A217" s="11"/>
+      <c r="B217" s="11"/>
     </row>
     <row r="218" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A218" s="12"/>
-      <c r="B218" s="12"/>
+      <c r="A218" s="11"/>
+      <c r="B218" s="11"/>
     </row>
     <row r="219" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A219" s="12"/>
-      <c r="B219" s="12"/>
+      <c r="A219" s="11"/>
+      <c r="B219" s="11"/>
     </row>
     <row r="220" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A220" s="12"/>
-      <c r="B220" s="12"/>
+      <c r="A220" s="11"/>
+      <c r="B220" s="11"/>
     </row>
     <row r="221" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A221" s="12"/>
-      <c r="B221" s="12"/>
+      <c r="A221" s="11"/>
+      <c r="B221" s="11"/>
     </row>
     <row r="222" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A222" s="12"/>
-      <c r="B222" s="12"/>
+      <c r="A222" s="11"/>
+      <c r="B222" s="11"/>
     </row>
     <row r="223" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A223" s="12"/>
-      <c r="B223" s="12"/>
+      <c r="A223" s="11"/>
+      <c r="B223" s="11"/>
     </row>
     <row r="224" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A224" s="12"/>
-      <c r="B224" s="12"/>
+      <c r="A224" s="11"/>
+      <c r="B224" s="11"/>
     </row>
     <row r="225" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A225" s="12"/>
-      <c r="B225" s="12"/>
+      <c r="A225" s="11"/>
+      <c r="B225" s="11"/>
     </row>
     <row r="226" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A226" s="12"/>
-      <c r="B226" s="12"/>
+      <c r="A226" s="11"/>
+      <c r="B226" s="11"/>
     </row>
     <row r="227" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A227" s="12"/>
-      <c r="B227" s="12"/>
+      <c r="A227" s="11"/>
+      <c r="B227" s="11"/>
     </row>
     <row r="228" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A228" s="12"/>
-      <c r="B228" s="12"/>
+      <c r="A228" s="11"/>
+      <c r="B228" s="11"/>
     </row>
     <row r="229" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A229" s="12"/>
-      <c r="B229" s="12"/>
+      <c r="A229" s="11"/>
+      <c r="B229" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>